<commit_message>
Agregado experto y modificados los anexos
</commit_message>
<xml_diff>
--- a/data/programs/piuh/docs/Anexo4.xlsx
+++ b/data/programs/piuh/docs/Anexo4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VRIP 2023\DCT\programa institucional\anexos evalaucion de expertos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F78312-B3FD-413A-9203-47E9FABEFE6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ED8C40-D89C-4F84-9AB0-8006400938A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8856" activeTab="1" xr2:uid="{69B21BFD-30A4-4AAC-962F-F68B9D4FBE39}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8856" xr2:uid="{69B21BFD-30A4-4AAC-962F-F68B9D4FBE39}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMEN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>CRITERIO 1 – CONTENIDO CIENTÍFICO-TECNOLÓGICO</t>
   </si>
@@ -154,15 +154,9 @@
     <t>l) Originalidad. Creación de nuevo conocimiento.</t>
   </si>
   <si>
-    <t>PLANILLA DE EVALUACIÓN DE PROYECTOS BÁSICOS y BÁSICOS APLICADOS</t>
-  </si>
-  <si>
     <t>f) Manejo del estado del conocimiento y de la experiencia previa en la temática del proyecto.</t>
   </si>
   <si>
-    <t>PLANILLA DE EVALUACIÓN DE PROYECTOS INVESTIGACIÓN BÁSICA Y BASICA APLICADA</t>
-  </si>
-  <si>
     <t>f) Correspondencia entre las actividades a desarrollar (el Plan deTrabajo) con la metodología planteada y los resultados esperados.</t>
   </si>
   <si>
@@ -176,6 +170,15 @@
   </si>
   <si>
     <t>CRITERIO 3 – POSIBILIDAD DE ÉXITO DEL PROYECTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLANILLA DE EVALUACIÓN DE PROYECTOS INVESTIGACIÓN BÁSICA </t>
+  </si>
+  <si>
+    <t>PLANILLA DE EVALUACIÓN DE PROYECTOS INVESTIGACIÓN BÁSICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLANILLA DE EVALUACIÓN DE PROYECTOS INVESTIGACIÓN  BÁSICA </t>
   </si>
 </sst>
 </file>
@@ -483,6 +486,33 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,39 +567,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -584,9 +590,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="12"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -904,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F77346-D265-4FEA-AA88-AC27BE821FC2}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,133 +919,127 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="C2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="14">
         <f>'Criterio 1'!D22+'Criterio 2'!D17+'Criterio 3'!D18+'Criterio 4'!D16</f>
-        <v>360</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="4">
         <f>F9/4</f>
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="40"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="38"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="41"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C11:C13"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C17:F19"/>
     <mergeCell ref="C9:E9"/>
@@ -1050,6 +1047,12 @@
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C11:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1059,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1959092A-2B11-4F9A-973A-CA9064AC0754}">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,10 +1073,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="33"/>
+      <c r="C2" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="44"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
@@ -1082,23 +1085,23 @@
       <c r="B4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="21"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1120,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1128,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1136,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1144,7 +1147,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1152,15 +1155,15 @@
         <v>7</v>
       </c>
       <c r="D15" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -1168,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -1176,7 +1179,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -1184,7 +1187,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -1192,7 +1195,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1200,7 +1203,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1208,7 +1211,7 @@
         <v>40</v>
       </c>
       <c r="D22" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1217,7 +1220,7 @@
       </c>
       <c r="D23">
         <f>SUM(D11:D22)/12</f>
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1238,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFD788B-2642-4F8F-9022-D931542E3BAB}">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,10 +1253,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="33"/>
+      <c r="C2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="44"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
@@ -1262,23 +1265,23 @@
       <c r="B4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="21"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1300,40 +1303,40 @@
         <v>14</v>
       </c>
       <c r="D11" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="44">
-        <v>90</v>
+      <c r="D12" s="45">
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="45"/>
+      <c r="D13" s="46"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="45"/>
+      <c r="D14" s="46"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="45"/>
+      <c r="D15" s="46"/>
     </row>
     <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="46"/>
+      <c r="D16" s="47"/>
     </row>
     <row r="17" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="6" t="s">
@@ -1341,7 +1344,7 @@
       </c>
       <c r="D17" s="4">
         <f>SUM(D11:D16)/2</f>
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1362,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC01D8BD-A22C-44DE-AA8B-F8E382C65BE8}">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:D9"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,10 +1377,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="49"/>
+      <c r="C2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="15"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
@@ -1386,28 +1389,28 @@
       <c r="B4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="21"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="43"/>
     </row>
@@ -1419,12 +1422,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -1432,15 +1435,15 @@
         <v>22</v>
       </c>
       <c r="D12" s="4">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
@@ -1448,31 +1451,31 @@
         <v>24</v>
       </c>
       <c r="D14" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1481,7 +1484,7 @@
       </c>
       <c r="D18" s="4">
         <f>SUM(D11:D17)/7</f>
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1501,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC80D5A-9992-4D67-929E-16A25727D0A7}">
   <dimension ref="B2:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,10 +1516,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="33"/>
+      <c r="C2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="44"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
@@ -1525,30 +1528,30 @@
       <c r="B4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="21"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="48"/>
+      <c r="C9" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="49"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
@@ -1563,7 +1566,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -1571,15 +1574,15 @@
         <v>26</v>
       </c>
       <c r="D12" s="4">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1587,15 +1590,15 @@
         <v>28</v>
       </c>
       <c r="D14" s="4">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1604,7 +1607,7 @@
       </c>
       <c r="D16" s="4">
         <f>SUM(D11:D15)/5</f>
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambiado Anexo 4 en PNCB
</commit_message>
<xml_diff>
--- a/data/programs/piuh/docs/Anexo4.xlsx
+++ b/data/programs/piuh/docs/Anexo4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VRIP 2023\DCT\programa institucional\anexos evalaucion de expertos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SALVA 19 MARZO\Desktop C\NUEVO PROGRAMA PNCBN\Evaluacion y seleccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ED8C40-D89C-4F84-9AB0-8006400938A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2A5D7B-480A-4ACF-807B-3E91F6EC9A03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8856" xr2:uid="{69B21BFD-30A4-4AAC-962F-F68B9D4FBE39}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{69B21BFD-30A4-4AAC-962F-F68B9D4FBE39}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMEN" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Criterio 3" sheetId="3" r:id="rId4"/>
     <sheet name="Criterio 4" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>CRITERIO 1 – CONTENIDO CIENTÍFICO-TECNOLÓGICO</t>
   </si>
@@ -55,6 +55,9 @@
     <t>e) Definición del alcance.</t>
   </si>
   <si>
+    <t>f) Manejodel estado del conocimiento y de la experiencia previa en la temática del proyecto.</t>
+  </si>
+  <si>
     <t>g) Metodología de trabajo propuesta para alcanzar los objetivos.</t>
   </si>
   <si>
@@ -73,9 +76,15 @@
     <t>CRITERIO 2 – PERTINENCIA DE LA PROPUESTA</t>
   </si>
   <si>
+    <t>a) Correspondencia de los objetivos del Proyecto con los objetivos del Programa</t>
+  </si>
+  <si>
     <t>b) Importancia del problema científico a abordar y aporte de la propuesta a su solución.</t>
   </si>
   <si>
+    <t>c)  Identificación de los clientes, usuarios o beneficiarios potencialesy/o reales del(os) resultado(s).</t>
+  </si>
+  <si>
     <t>d) Posibles impactos:</t>
   </si>
   <si>
@@ -94,6 +103,12 @@
     <t>Calificación promedio:</t>
   </si>
   <si>
+    <t>CRITERIO 3 – PROBABILIDAD DE ÉXITO DEL PROYECTO</t>
+  </si>
+  <si>
+    <t>a) Valoración de la idoneidad de la institución ejecutora y la (s) participante(s).</t>
+  </si>
+  <si>
     <t>b) Valoración de la idoneidad del equipo de investigación.</t>
   </si>
   <si>
@@ -106,6 +121,21 @@
     <t>e) Medios materiales requeridos para la ejecución del Proyecto, en poder de las instituciones participantes y pendientes de adquirir.</t>
   </si>
   <si>
+    <t>f)  Valoración acerca de los riesgos reales y posibles que pueda confrontar el proyecto. Flexibilidad del diseño para adaptarse al cambio de las condiciones concretas durante su ejecución.</t>
+  </si>
+  <si>
+    <t>g) Correspondencia entre las actividades a desarrollar (el Plan deTrabajo) con la metodología planteada y los resultados esperados.</t>
+  </si>
+  <si>
+    <t>h) Coherencia entre las actividades propuestas y los plazos establecidos para su ejecución.</t>
+  </si>
+  <si>
+    <t>i) Valoración sobre el monto y estructura del presupuesto solicitado para la investigación.</t>
+  </si>
+  <si>
+    <t>CRITERIO 4 – PROBABILIDAD DE CONTINUIDAD</t>
+  </si>
+  <si>
     <t>a) Generación de proyectos aplicados o de desarrollo a partir de los resultados previstos.</t>
   </si>
   <si>
@@ -142,6 +172,9 @@
     <t>Título del Proyecto:</t>
   </si>
   <si>
+    <t>PLANILLA DE EVALUACIÓN DE PROYECTOS BÁSICOS</t>
+  </si>
+  <si>
     <t>Nombre del Evaluador</t>
   </si>
   <si>
@@ -154,31 +187,10 @@
     <t>l) Originalidad. Creación de nuevo conocimiento.</t>
   </si>
   <si>
-    <t>f) Manejo del estado del conocimiento y de la experiencia previa en la temática del proyecto.</t>
-  </si>
-  <si>
-    <t>f) Correspondencia entre las actividades a desarrollar (el Plan deTrabajo) con la metodología planteada y los resultados esperados.</t>
-  </si>
-  <si>
-    <t>g) Coherencia entre las actividades propuestas y los plazos establecidos para su ejecución.</t>
-  </si>
-  <si>
-    <t>h) Valoración sobre el monto y estructura del presupuesto solicitado para la investigación.</t>
-  </si>
-  <si>
-    <t>CRITERIO 4 – POSIBILIDAD  DE CONTINUIDAD</t>
-  </si>
-  <si>
-    <t>CRITERIO 3 – POSIBILIDAD DE ÉXITO DEL PROYECTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLANILLA DE EVALUACIÓN DE PROYECTOS INVESTIGACIÓN BÁSICA </t>
-  </si>
-  <si>
-    <t>PLANILLA DE EVALUACIÓN DE PROYECTOS INVESTIGACIÓN BÁSICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLANILLA DE EVALUACIÓN DE PROYECTOS INVESTIGACIÓN  BÁSICA </t>
+    <t>INTELIGENCIA ARTIFICIAL APLICADA. ESPECTROSCOPÍA Y BIOACTIVIDAD</t>
+  </si>
+  <si>
+    <t>Modelación de la habitabilidad de ecosistemas cubanos</t>
   </si>
 </sst>
 </file>
@@ -446,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -486,8 +498,68 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -513,68 +585,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -907,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F77346-D265-4FEA-AA88-AC27BE821FC2}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -919,127 +934,137 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="C2" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="C4" s="31">
+        <v>67</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
+        <v>46</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="30"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="24"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
+      <c r="C9" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="14">
-        <f>'Criterio 1'!D22+'Criterio 2'!D17+'Criterio 3'!D18+'Criterio 4'!D16</f>
-        <v>400</v>
+        <f>'Criterio 1'!D24+'Criterio 2'!D19+'Criterio 3'!D20+'Criterio 4'!D16</f>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
+      <c r="C10" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
       <c r="F10" s="4">
         <f>F9/4</f>
-        <v>100</v>
+        <v>92.75</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="21" t="s">
-        <v>34</v>
+      <c r="C11" s="41" t="s">
+        <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
+        <v>41</v>
+      </c>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="22"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="23"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
+        <v>48</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
+        <v>49</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C11:C13"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C17:F19"/>
     <mergeCell ref="C9:E9"/>
@@ -1047,12 +1072,6 @@
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C11:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1060,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1959092A-2B11-4F9A-973A-CA9064AC0754}">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,42 +1092,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="44"/>
+      <c r="C2" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="35"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="29"/>
+        <v>46</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="30"/>
-      <c r="D6" s="32"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="33"/>
-      <c r="D7" s="35"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="45"/>
     </row>
     <row r="10" spans="2:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
@@ -1123,7 +1144,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1131,7 +1152,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1139,7 +1160,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1147,7 +1168,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1155,72 +1176,75 @@
         <v>7</v>
       </c>
       <c r="D15" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D16" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D19" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="3" t="s">
-        <v>11</v>
+      <c r="C20" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="D20" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="3" t="s">
-        <v>40</v>
+      <c r="C22" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="D22" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24">
         <f>SUM(D11:D22)/12</f>
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1239,56 +1263,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFD788B-2642-4F8F-9022-D931542E3BAB}">
-  <dimension ref="B2:F17"/>
+  <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="59.77734375" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="44"/>
+      <c r="C2" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="35"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="29"/>
+        <v>46</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="30"/>
-      <c r="D6" s="32"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="33"/>
-      <c r="D7" s="35"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="43"/>
+      <c r="C9" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="45"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
@@ -1300,57 +1326,73 @@
     </row>
     <row r="11" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="46"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="7" t="s">
+      <c r="D12" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="46"/>
+      <c r="D13" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="46">
+        <v>90</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="46"/>
-    </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="D15" s="47"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="D16" s="47"/>
     </row>
-    <row r="17" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="4">
-        <f>SUM(D11:D16)/2</f>
-        <v>100</v>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="47"/>
+    </row>
+    <row r="18" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="48"/>
+    </row>
+    <row r="19" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4">
+        <f>SUM(D11:D18)/4</f>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="D14:D18"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
@@ -1363,56 +1405,58 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC01D8BD-A22C-44DE-AA8B-F8E382C65BE8}">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="58.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="29"/>
+        <v>46</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="30"/>
-      <c r="D6" s="32"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="33"/>
-      <c r="D7" s="35"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="43"/>
+      <c r="C9" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="45"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
@@ -1422,9 +1466,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D11" s="4">
         <v>100</v>
@@ -1432,15 +1476,15 @@
     </row>
     <row r="12" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4">
         <v>100</v>
@@ -1448,7 +1492,7 @@
     </row>
     <row r="14" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4">
         <v>100</v>
@@ -1456,35 +1500,51 @@
     </row>
     <row r="15" spans="2:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D16" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D17" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="6" t="s">
-        <v>20</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D18" s="4">
-        <f>SUM(D11:D17)/7</f>
-        <v>100</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4">
+        <f>SUM(D11:D18)/8</f>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1504,54 +1564,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC80D5A-9992-4D67-929E-16A25727D0A7}">
   <dimension ref="B2:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="62" customWidth="1"/>
+    <col min="3" max="3" width="51.109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="44"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="29"/>
+        <v>46</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="30"/>
-      <c r="D6" s="32"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="33"/>
-      <c r="D7" s="35"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="49"/>
+      <c r="C9" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="50"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
@@ -1563,7 +1625,7 @@
     </row>
     <row r="11" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D11" s="4">
         <v>100</v>
@@ -1571,43 +1633,43 @@
     </row>
     <row r="12" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D12" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D13" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D14" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D16" s="4">
         <f>SUM(D11:D15)/5</f>
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>